<commit_message>
rename admission into enrollment
</commit_message>
<xml_diff>
--- a/EnrollmentSystem.xlsx
+++ b/EnrollmentSystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keyzer-Soze\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keyzer-Soze\Documents\GitHub\EnrollmentSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D849FE9-4456-4C53-9312-05DE53738929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E2E4D3-EEFE-4FDF-B5B0-4A3462BC934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59E22794-A3F1-4942-982E-D4AE5AE1804D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{59E22794-A3F1-4942-982E-D4AE5AE1804D}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>2022-01-001</t>
   </si>
@@ -48,9 +48,6 @@
 For Transferee: Transcript of Record Notice of Admission Medical Clearance Application Form Cert of transfer</t>
   </si>
   <si>
-    <t>year to enroll dropdown</t>
-  </si>
-  <si>
     <t>Accept enrollments</t>
   </si>
   <si>
@@ -67,6 +64,30 @@
   </si>
   <si>
     <t>enrollment-system-of-cvsu-silang-campus</t>
+  </si>
+  <si>
+    <t>complete uploading files and approved, before download link available</t>
+  </si>
+  <si>
+    <t>add year level</t>
+  </si>
+  <si>
+    <t>add school year</t>
+  </si>
+  <si>
+    <t>add profile picture</t>
+  </si>
+  <si>
+    <t>registrar will upload reg form in admin page</t>
+  </si>
+  <si>
+    <t>auto-copy info from previous enrollment</t>
+  </si>
+  <si>
+    <t>rename records to enrollments</t>
+  </si>
+  <si>
+    <t>add filtering by school year and by course</t>
   </si>
 </sst>
 </file>
@@ -128,6 +149,314 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>560582</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>132557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C785DDB6-28E8-C315-DD8A-77690A2B640A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2219325" y="838200"/>
+          <a:ext cx="11142857" cy="6342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>598731</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>75450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC90FB8D-42B4-AD50-34E9-3629E7E35D49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="819150" y="171450"/>
+          <a:ext cx="10752381" cy="6000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7B47ABE-B387-45CB-89AD-DC300EBFC5D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1676400" y="1504950"/>
+          <a:ext cx="7543800" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>321450</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>16650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>550050</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>169050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A75F702-80B8-C769-608E-F0596931420A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8341500" y="6750825"/>
+          <a:ext cx="7543800" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>55016</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBB1898E-730E-2FD3-63E6-E3287672D7C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="4895850"/>
+          <a:ext cx="7772400" cy="4369841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA984F60-44CD-4E70-AA52-6DD4E23E16D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8324850" y="285750"/>
+          <a:ext cx="7772400" cy="5829300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,20 +758,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345B29BE-3DF3-453F-A36C-96CBEC28E948}">
   <dimension ref="B4:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -450,11 +779,12 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -463,21 +793,22 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063071C1-92CC-4E26-B8E9-BD5A583240DB}">
-  <dimension ref="D5"/>
+  <dimension ref="D4:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,63 +816,101 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="5" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F4FF6F-AB13-4DE6-8CC6-CB7CD1440FC0}">
-  <dimension ref="D5"/>
+  <dimension ref="A4:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:4" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4FF08A-3656-475F-90FA-6A8AA80F9D5A}">
-  <dimension ref="C7:C9"/>
+  <dimension ref="C7:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added layout in account page
</commit_message>
<xml_diff>
--- a/EnrollmentSystem.xlsx
+++ b/EnrollmentSystem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keyzer-Soze\Documents\GitHub\EnrollmentSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E2E4D3-EEFE-4FDF-B5B0-4A3462BC934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D44CA8-3184-4977-8FB8-D2840ADD03CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{59E22794-A3F1-4942-982E-D4AE5AE1804D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{59E22794-A3F1-4942-982E-D4AE5AE1804D}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -807,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063071C1-92CC-4E26-B8E9-BD5A583240DB}">
   <dimension ref="D4:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F4FF6F-AB13-4DE6-8CC6-CB7CD1440FC0}">
   <dimension ref="A4:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4FF08A-3656-475F-90FA-6A8AA80F9D5A}">
   <dimension ref="C7:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>